<commit_message>
Se añadio bucle de productos
</commit_message>
<xml_diff>
--- a/Excel_Factura_prueba_0020.xlsx
+++ b/Excel_Factura_prueba_0020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Perfil\Rogers Allan Merchan Sepulveda\Descargas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Perfil\Rogers Allan Merchan Sepulveda\Escritorio\BotHealthyBeta01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700A4420-F53D-404C-AC1E-71A697028AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A965E9-3E51-44C0-A6CD-9CB85D802FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>